<commit_message>
Added aspects and classifications for inserting LCI data, fixed typos.
</commit_message>
<xml_diff>
--- a/IEDC_Classification_fill/age_cohort_ranges_data.xlsx
+++ b/IEDC_Classification_fill/age_cohort_ranges_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>2000-2010</t>
+  </si>
+  <si>
+    <t>2010-2015</t>
+  </si>
+  <si>
+    <t>1993-2002</t>
+  </si>
+  <si>
+    <t>2002-2003</t>
+  </si>
+  <si>
+    <t>1992-2002</t>
   </si>
 </sst>
 </file>
@@ -176,12 +188,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -491,10 +506,13 @@
   <dimension ref="A1:T101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F101"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -857,8 +875,8 @@
       <c r="C22" s="2">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>20</v>
+      <c r="F22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,8 +889,8 @@
       <c r="C23" s="2">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>20</v>
+      <c r="F23" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -885,8 +903,8 @@
       <c r="C24" s="2">
         <v>0</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>20</v>
+      <c r="F24" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -899,8 +917,8 @@
       <c r="C25" s="2">
         <v>0</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>20</v>
+      <c r="F25" s="5">
+        <v>2003</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -913,8 +931,8 @@
       <c r="C26" s="2">
         <v>0</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>20</v>
+      <c r="F26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added classification items for uploading 10 more datasets.
</commit_message>
<xml_diff>
--- a/IEDC_Classification_fill/age_cohort_ranges_data.xlsx
+++ b/IEDC_Classification_fill/age_cohort_ranges_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -146,6 +146,42 @@
   </si>
   <si>
     <t>1992-2002</t>
+  </si>
+  <si>
+    <t>1999-2003</t>
+  </si>
+  <si>
+    <t>ca. 2010</t>
+  </si>
+  <si>
+    <t>ca. 2005</t>
+  </si>
+  <si>
+    <t>ca. 2000</t>
+  </si>
+  <si>
+    <t>ca. 2001</t>
+  </si>
+  <si>
+    <t>ca. 2002</t>
+  </si>
+  <si>
+    <t>ca. 2003</t>
+  </si>
+  <si>
+    <t>ca. 2004</t>
+  </si>
+  <si>
+    <t>ca. 2006</t>
+  </si>
+  <si>
+    <t>ca. 2007</t>
+  </si>
+  <si>
+    <t>ca. 2008</t>
+  </si>
+  <si>
+    <t>ca. 2009</t>
   </si>
 </sst>
 </file>
@@ -503,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T101"/>
+  <dimension ref="A1:T201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -959,8 +995,8 @@
       <c r="C28" s="2">
         <v>0</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>20</v>
+      <c r="F28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -973,8 +1009,8 @@
       <c r="C29" s="2">
         <v>0</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>20</v>
+      <c r="F29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -987,8 +1023,8 @@
       <c r="C30" s="2">
         <v>0</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>20</v>
+      <c r="F30" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1001,8 +1037,8 @@
       <c r="C31" s="2">
         <v>0</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>20</v>
+      <c r="F31" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1015,8 +1051,8 @@
       <c r="C32" s="2">
         <v>0</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>20</v>
+      <c r="F32" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1029,8 +1065,8 @@
       <c r="C33" s="2">
         <v>0</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>20</v>
+      <c r="F33" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1043,8 +1079,8 @@
       <c r="C34" s="2">
         <v>0</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>20</v>
+      <c r="F34" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,8 +1093,8 @@
       <c r="C35" s="2">
         <v>0</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>20</v>
+      <c r="F35" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1071,8 +1107,8 @@
       <c r="C36" s="2">
         <v>0</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>20</v>
+      <c r="F36" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1085,8 +1121,8 @@
       <c r="C37" s="2">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>20</v>
+      <c r="F37" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1099,8 +1135,8 @@
       <c r="C38" s="2">
         <v>0</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>20</v>
+      <c r="F38" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1982,6 +2018,1406 @@
         <v>0</v>
       </c>
       <c r="F101" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="2">
+        <v>14</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="2">
+        <v>14</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="2">
+        <v>14</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="2">
+        <v>14</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="2">
+        <v>14</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="2">
+        <v>14</v>
+      </c>
+      <c r="C107" s="2">
+        <v>0</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="2">
+        <v>14</v>
+      </c>
+      <c r="C108" s="2">
+        <v>0</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="2">
+        <v>14</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2">
+        <v>14</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="2">
+        <v>14</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2">
+        <v>14</v>
+      </c>
+      <c r="C112" s="2">
+        <v>0</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="2">
+        <v>14</v>
+      </c>
+      <c r="C113" s="2">
+        <v>0</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="2">
+        <v>14</v>
+      </c>
+      <c r="C114" s="2">
+        <v>0</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="2">
+        <v>14</v>
+      </c>
+      <c r="C115" s="2">
+        <v>0</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="2">
+        <v>14</v>
+      </c>
+      <c r="C116" s="2">
+        <v>0</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="2">
+        <v>14</v>
+      </c>
+      <c r="C117" s="2">
+        <v>0</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="2">
+        <v>14</v>
+      </c>
+      <c r="C118" s="2">
+        <v>0</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="2">
+        <v>14</v>
+      </c>
+      <c r="C119" s="2">
+        <v>0</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="2">
+        <v>14</v>
+      </c>
+      <c r="C120" s="2">
+        <v>0</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="2">
+        <v>14</v>
+      </c>
+      <c r="C121" s="2">
+        <v>0</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="2">
+        <v>14</v>
+      </c>
+      <c r="C122" s="2">
+        <v>0</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="2">
+        <v>14</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="2">
+        <v>14</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="2">
+        <v>14</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="2">
+        <v>14</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="2">
+        <v>14</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="2">
+        <v>14</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="2">
+        <v>14</v>
+      </c>
+      <c r="C129" s="2">
+        <v>0</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="2">
+        <v>14</v>
+      </c>
+      <c r="C130" s="2">
+        <v>0</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="2">
+        <v>14</v>
+      </c>
+      <c r="C131" s="2">
+        <v>0</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="2">
+        <v>14</v>
+      </c>
+      <c r="C132" s="2">
+        <v>0</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2">
+        <v>14</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="2">
+        <v>14</v>
+      </c>
+      <c r="C134" s="2">
+        <v>0</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="2">
+        <v>14</v>
+      </c>
+      <c r="C135" s="2">
+        <v>0</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="2">
+        <v>14</v>
+      </c>
+      <c r="C136" s="2">
+        <v>0</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="2">
+        <v>14</v>
+      </c>
+      <c r="C137" s="2">
+        <v>0</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="2">
+        <v>14</v>
+      </c>
+      <c r="C138" s="2">
+        <v>0</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="2">
+        <v>14</v>
+      </c>
+      <c r="C139" s="2">
+        <v>0</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="2">
+        <v>14</v>
+      </c>
+      <c r="C140" s="2">
+        <v>0</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="2">
+        <v>14</v>
+      </c>
+      <c r="C141" s="2">
+        <v>0</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="2">
+        <v>14</v>
+      </c>
+      <c r="C142" s="2">
+        <v>0</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="2">
+        <v>14</v>
+      </c>
+      <c r="C143" s="2">
+        <v>0</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="2">
+        <v>14</v>
+      </c>
+      <c r="C144" s="2">
+        <v>0</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" s="2">
+        <v>14</v>
+      </c>
+      <c r="C145" s="2">
+        <v>0</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" s="2">
+        <v>14</v>
+      </c>
+      <c r="C146" s="2">
+        <v>0</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" s="2">
+        <v>14</v>
+      </c>
+      <c r="C147" s="2">
+        <v>0</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" s="2">
+        <v>14</v>
+      </c>
+      <c r="C148" s="2">
+        <v>0</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" s="2">
+        <v>14</v>
+      </c>
+      <c r="C149" s="2">
+        <v>0</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="2">
+        <v>14</v>
+      </c>
+      <c r="C150" s="2">
+        <v>0</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" s="2">
+        <v>14</v>
+      </c>
+      <c r="C151" s="2">
+        <v>0</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" s="2">
+        <v>14</v>
+      </c>
+      <c r="C152" s="2">
+        <v>0</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" s="2">
+        <v>14</v>
+      </c>
+      <c r="C153" s="2">
+        <v>0</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" s="2">
+        <v>14</v>
+      </c>
+      <c r="C154" s="2">
+        <v>0</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" s="2">
+        <v>14</v>
+      </c>
+      <c r="C155" s="2">
+        <v>0</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" s="2">
+        <v>14</v>
+      </c>
+      <c r="C156" s="2">
+        <v>0</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="2">
+        <v>14</v>
+      </c>
+      <c r="C157" s="2">
+        <v>0</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="2">
+        <v>14</v>
+      </c>
+      <c r="C158" s="2">
+        <v>0</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" s="2">
+        <v>14</v>
+      </c>
+      <c r="C159" s="2">
+        <v>0</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" s="2">
+        <v>14</v>
+      </c>
+      <c r="C160" s="2">
+        <v>0</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" s="2">
+        <v>14</v>
+      </c>
+      <c r="C161" s="2">
+        <v>0</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" s="2">
+        <v>14</v>
+      </c>
+      <c r="C162" s="2">
+        <v>0</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" s="2">
+        <v>14</v>
+      </c>
+      <c r="C163" s="2">
+        <v>0</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" s="2">
+        <v>14</v>
+      </c>
+      <c r="C164" s="2">
+        <v>0</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" s="2">
+        <v>14</v>
+      </c>
+      <c r="C165" s="2">
+        <v>0</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" s="2">
+        <v>14</v>
+      </c>
+      <c r="C166" s="2">
+        <v>0</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" s="2">
+        <v>14</v>
+      </c>
+      <c r="C167" s="2">
+        <v>0</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" s="2">
+        <v>14</v>
+      </c>
+      <c r="C168" s="2">
+        <v>0</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" s="2">
+        <v>14</v>
+      </c>
+      <c r="C169" s="2">
+        <v>0</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" s="2">
+        <v>14</v>
+      </c>
+      <c r="C170" s="2">
+        <v>0</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" s="2">
+        <v>14</v>
+      </c>
+      <c r="C171" s="2">
+        <v>0</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" s="2">
+        <v>14</v>
+      </c>
+      <c r="C172" s="2">
+        <v>0</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" s="2">
+        <v>14</v>
+      </c>
+      <c r="C173" s="2">
+        <v>0</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" s="2">
+        <v>14</v>
+      </c>
+      <c r="C174" s="2">
+        <v>0</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" s="2">
+        <v>14</v>
+      </c>
+      <c r="C175" s="2">
+        <v>0</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" s="2">
+        <v>14</v>
+      </c>
+      <c r="C176" s="2">
+        <v>0</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" s="2">
+        <v>14</v>
+      </c>
+      <c r="C177" s="2">
+        <v>0</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" s="2">
+        <v>14</v>
+      </c>
+      <c r="C178" s="2">
+        <v>0</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" s="2">
+        <v>14</v>
+      </c>
+      <c r="C179" s="2">
+        <v>0</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" s="2">
+        <v>14</v>
+      </c>
+      <c r="C180" s="2">
+        <v>0</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" s="2">
+        <v>14</v>
+      </c>
+      <c r="C181" s="2">
+        <v>0</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" s="2">
+        <v>14</v>
+      </c>
+      <c r="C182" s="2">
+        <v>0</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" s="2">
+        <v>14</v>
+      </c>
+      <c r="C183" s="2">
+        <v>0</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" s="2">
+        <v>14</v>
+      </c>
+      <c r="C184" s="2">
+        <v>0</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" s="2">
+        <v>14</v>
+      </c>
+      <c r="C185" s="2">
+        <v>0</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" s="2">
+        <v>14</v>
+      </c>
+      <c r="C186" s="2">
+        <v>0</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" s="2">
+        <v>14</v>
+      </c>
+      <c r="C187" s="2">
+        <v>0</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" s="2">
+        <v>14</v>
+      </c>
+      <c r="C188" s="2">
+        <v>0</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" s="2">
+        <v>14</v>
+      </c>
+      <c r="C189" s="2">
+        <v>0</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" s="2">
+        <v>14</v>
+      </c>
+      <c r="C190" s="2">
+        <v>0</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" s="2">
+        <v>14</v>
+      </c>
+      <c r="C191" s="2">
+        <v>0</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" s="2">
+        <v>14</v>
+      </c>
+      <c r="C192" s="2">
+        <v>0</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" s="2">
+        <v>14</v>
+      </c>
+      <c r="C193" s="2">
+        <v>0</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" s="2">
+        <v>14</v>
+      </c>
+      <c r="C194" s="2">
+        <v>0</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" s="2">
+        <v>14</v>
+      </c>
+      <c r="C195" s="2">
+        <v>0</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" s="2">
+        <v>14</v>
+      </c>
+      <c r="C196" s="2">
+        <v>0</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" s="2">
+        <v>14</v>
+      </c>
+      <c r="C197" s="2">
+        <v>0</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" s="2">
+        <v>14</v>
+      </c>
+      <c r="C198" s="2">
+        <v>0</v>
+      </c>
+      <c r="F198" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" s="2">
+        <v>14</v>
+      </c>
+      <c r="C199" s="2">
+        <v>0</v>
+      </c>
+      <c r="F199" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" s="2">
+        <v>14</v>
+      </c>
+      <c r="C200" s="2">
+        <v>0</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" s="2">
+        <v>14</v>
+      </c>
+      <c r="C201" s="2">
+        <v>0</v>
+      </c>
+      <c r="F201" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>